<commit_message>
Update Conn DB & Docs
</commit_message>
<xml_diff>
--- a/RECURSOS GENERALES/DOCUMENTOS/TABLAS -  BASE de DATOS.xlsx
+++ b/RECURSOS GENERALES/DOCUMENTOS/TABLAS -  BASE de DATOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27806"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27528"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a32049e1d288c0c2/Media Técnica/PROYECTOS DE GRADO/INDENETWORK/IndeNetwork GITHUB/IndeNetwork/RECURSOS GENERALES/DOCUMENTOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maico\Dropbox\PROYECTO DE GRADO\INDENETWORK\IndeNetwork - Repositorio\IndeNetwork\RECURSOS GENERALES\DOCUMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FD18E73-2665-4892-83A1-9425D455793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8A8228-D172-4EEE-B362-DB5A2DC391FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4385422B-F3FD-48BA-9071-C2901DFECF3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4385422B-F3FD-48BA-9071-C2901DFECF3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>id_profesor</t>
   </si>
@@ -128,9 +128,6 @@
     <t>fk_miembro2</t>
   </si>
   <si>
-    <t>estado_amigo</t>
-  </si>
-  <si>
     <t>tipo_miembro</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>id_publicacion</t>
   </si>
   <si>
-    <t>fk_publicador</t>
-  </si>
-  <si>
     <t>texto_publicacion</t>
   </si>
   <si>
@@ -167,9 +161,6 @@
     <t>MIEMBROS</t>
   </si>
   <si>
-    <t>fk_tipoMiembro</t>
-  </si>
-  <si>
     <t>fechaHora_miembro</t>
   </si>
   <si>
@@ -252,6 +243,12 @@
   </si>
   <si>
     <t>texto_comTarea</t>
+  </si>
+  <si>
+    <t>fk_profesor</t>
+  </si>
+  <si>
+    <t>fk_estudiante</t>
   </si>
 </sst>
 </file>
@@ -297,13 +294,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1016,26 +1013,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1066,130 +1063,130 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{17DACAE4-AD98-4D4F-BC71-3F02BF3A87B9}" name="Tabla1" displayName="Tabla1" ref="A1:A6" totalsRowShown="0" headerRowDxfId="37" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{17DACAE4-AD98-4D4F-BC71-3F02BF3A87B9}" name="Tabla1" displayName="Tabla1" ref="A1:A6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A1:A6" xr:uid="{17DACAE4-AD98-4D4F-BC71-3F02BF3A87B9}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{8ED60697-4798-4A21-839B-09D4A402A67E}" name="PROFESORES" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{8ED60697-4798-4A21-839B-09D4A402A67E}" name="PROFESORES" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6E0EB00D-03B1-45A4-A297-C053AD557C64}" name="Tabla11" displayName="Tabla11" ref="E13:E18" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6E0EB00D-03B1-45A4-A297-C053AD557C64}" name="Tabla11" displayName="Tabla11" ref="E13:E18" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="E13:E18" xr:uid="{6E0EB00D-03B1-45A4-A297-C053AD557C64}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A7717D4D-8008-4372-A8ED-D9692ADF6E33}" name="MENSAJES" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{A7717D4D-8008-4372-A8ED-D9692ADF6E33}" name="MENSAJES" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9EE101A7-5280-49D3-B7D3-A7D40D647307}" name="Tabla12" displayName="Tabla12" ref="G7:G10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
-  <autoFilter ref="G7:G10" xr:uid="{9EE101A7-5280-49D3-B7D3-A7D40D647307}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9EE101A7-5280-49D3-B7D3-A7D40D647307}" name="Tabla12" displayName="Tabla12" ref="G8:G11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="G8:G11" xr:uid="{9EE101A7-5280-49D3-B7D3-A7D40D647307}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{ADE195DF-FE46-409A-9DA8-E7E77A8379F0}" name="INTEGRANTES" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{ADE195DF-FE46-409A-9DA8-E7E77A8379F0}" name="INTEGRANTES" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{E919728C-5382-4295-B058-820167072F0F}" name="Tabla13" displayName="Tabla13" ref="G12:G20" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
-  <autoFilter ref="G12:G20" xr:uid="{E919728C-5382-4295-B058-820167072F0F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{E919728C-5382-4295-B058-820167072F0F}" name="Tabla13" displayName="Tabla13" ref="G13:G21" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="G13:G21" xr:uid="{E919728C-5382-4295-B058-820167072F0F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B892004B-6050-444C-9204-C902652F2C25}" name="TAREAS" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{B892004B-6050-444C-9204-C902652F2C25}" name="TAREAS" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{BD797C58-60A4-42AF-82FF-A99E8C7654ED}" name="Tabla14" displayName="Tabla14" ref="E20:E26" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="E20:E26" xr:uid="{BD797C58-60A4-42AF-82FF-A99E8C7654ED}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{BD797C58-60A4-42AF-82FF-A99E8C7654ED}" name="Tabla14" displayName="Tabla14" ref="I1:I7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="I1:I7" xr:uid="{BD797C58-60A4-42AF-82FF-A99E8C7654ED}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{EBA75B76-D335-478B-BCDD-2DFE0DBAF0C1}" name="COM_TAREA" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EBA75B76-D335-478B-BCDD-2DFE0DBAF0C1}" name="COM_TAREA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4664AAF0-0206-4AD3-A76E-D2126BC237F9}" name="Tabla2" displayName="Tabla2" ref="C1:C8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4664AAF0-0206-4AD3-A76E-D2126BC237F9}" name="Tabla2" displayName="Tabla2" ref="C1:C8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="C1:C8" xr:uid="{4664AAF0-0206-4AD3-A76E-D2126BC237F9}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1E39E60C-4420-4F5A-AF5A-1B5C8447012B}" name="ESTUDIANTES" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{1E39E60C-4420-4F5A-AF5A-1B5C8447012B}" name="ESTUDIANTES" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5EDB433F-1309-4582-909A-9C5E57C14F48}" name="Tabla3" displayName="Tabla3" ref="A8:A11" totalsRowShown="0" headerRowDxfId="33" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5EDB433F-1309-4582-909A-9C5E57C14F48}" name="Tabla3" displayName="Tabla3" ref="A8:A11" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A8:A11" xr:uid="{5EDB433F-1309-4582-909A-9C5E57C14F48}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9FF533FE-0A8E-40BD-A4FC-EF812E324618}" name="GRADOS" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{9FF533FE-0A8E-40BD-A4FC-EF812E324618}" name="GRADOS" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5D3B845F-C85C-4AE1-847D-B31D9D364C8C}" name="Tabla4" displayName="Tabla4" ref="E1:E7" totalsRowShown="0" headerRowDxfId="31" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5D3B845F-C85C-4AE1-847D-B31D9D364C8C}" name="Tabla4" displayName="Tabla4" ref="E1:E7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="E1:E7" xr:uid="{5D3B845F-C85C-4AE1-847D-B31D9D364C8C}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1F948F6B-67DB-422C-A586-1D4A9D47523A}" name="GRUPOS" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{1F948F6B-67DB-422C-A586-1D4A9D47523A}" name="GRUPOS" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{09223C19-37EE-4B3C-B533-93155494CFA3}" name="Tabla5" displayName="Tabla5" ref="E9:E11" totalsRowShown="0" headerRowDxfId="29" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{09223C19-37EE-4B3C-B533-93155494CFA3}" name="Tabla5" displayName="Tabla5" ref="E9:E11" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="E9:E11" xr:uid="{09223C19-37EE-4B3C-B533-93155494CFA3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3F1F31BA-A1EC-4C02-B4D8-2FC9863D99E0}" name="ASIGNATURAS" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{3F1F31BA-A1EC-4C02-B4D8-2FC9863D99E0}" name="ASIGNATURAS" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EDCE38D1-0D54-4561-890C-FF2E1FEF8A5D}" name="Tabla6" displayName="Tabla6" ref="C10:C15" totalsRowShown="0" headerRowDxfId="27" dataDxfId="28">
-  <autoFilter ref="C10:C15" xr:uid="{EDCE38D1-0D54-4561-890C-FF2E1FEF8A5D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EDCE38D1-0D54-4561-890C-FF2E1FEF8A5D}" name="Tabla6" displayName="Tabla6" ref="C10:C14" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="C10:C14" xr:uid="{EDCE38D1-0D54-4561-890C-FF2E1FEF8A5D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D0B4A2F4-50E8-4029-BA35-FA1874266703}" name="AMIGOS" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{D0B4A2F4-50E8-4029-BA35-FA1874266703}" name="AMIGOS" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43B26D67-69C7-4C84-9010-F969D077C774}" name="Tabla8" displayName="Tabla8" ref="A13:A19" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43B26D67-69C7-4C84-9010-F969D077C774}" name="Tabla8" displayName="Tabla8" ref="A13:A19" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A13:A19" xr:uid="{43B26D67-69C7-4C84-9010-F969D077C774}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{238792A1-4C08-4E3E-A4F7-862AE1B8A31F}" name="PUBLICACIONES" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{238792A1-4C08-4E3E-A4F7-862AE1B8A31F}" name="PUBLICACIONES" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{16CC5699-4573-4ABE-A286-7C00EB07445D}" name="Tabla9" displayName="Tabla9" ref="C17:C23" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
-  <autoFilter ref="C17:C23" xr:uid="{16CC5699-4573-4ABE-A286-7C00EB07445D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{16CC5699-4573-4ABE-A286-7C00EB07445D}" name="Tabla9" displayName="Tabla9" ref="C16:C22" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="C16:C22" xr:uid="{16CC5699-4573-4ABE-A286-7C00EB07445D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{86EDE893-AECC-4228-A63E-C63E1887DFC3}" name="COM_PUBLICACION" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{86EDE893-AECC-4228-A63E-C63E1887DFC3}" name="COM_PUBLICACION" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{37E64DA8-0107-43CB-81F5-E280262A46B8}" name="Tabla10" displayName="Tabla10" ref="G1:G5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13">
-  <autoFilter ref="G1:G5" xr:uid="{37E64DA8-0107-43CB-81F5-E280262A46B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{37E64DA8-0107-43CB-81F5-E280262A46B8}" name="Tabla10" displayName="Tabla10" ref="G1:G6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="G1:G6" xr:uid="{37E64DA8-0107-43CB-81F5-E280262A46B8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1FB7CA99-BE97-4002-B0CD-8127F2CDC399}" name="MIEMBROS" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{1FB7CA99-BE97-4002-B0CD-8127F2CDC399}" name="MIEMBROS" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1512,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5836246-8BCD-47E2-84AB-56902646E67F}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,363 +1528,285 @@
     <col min="9" max="16384" width="25.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2"/>
       <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2"/>
       <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="2"/>
+      <c r="E3" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="2"/>
       <c r="G14" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reubicación de Archivos, Modificaciones pequeñas en Archivos
</commit_message>
<xml_diff>
--- a/RECURSOS GENERALES/DOCUMENTOS/TABLAS -  BASE de DATOS.xlsx
+++ b/RECURSOS GENERALES/DOCUMENTOS/TABLAS -  BASE de DATOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28105"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maico\Dropbox\PROYECTO DE GRADO\INDENETWORK\IndeNetwork - Repositorio\IndeNetwork\RECURSOS GENERALES\DOCUMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8A8228-D172-4EEE-B362-DB5A2DC391FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31265937-2C68-47E2-8A67-6E225CEC0084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4385422B-F3FD-48BA-9071-C2901DFECF3A}"/>
+    <workbookView xWindow="10140" yWindow="105" windowWidth="10455" windowHeight="10800" xr2:uid="{4385422B-F3FD-48BA-9071-C2901DFECF3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>id_profesor</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>MIEMBROS</t>
-  </si>
-  <si>
-    <t>fechaHora_miembro</t>
   </si>
   <si>
     <t>fechaHora_grupo</t>
@@ -292,15 +289,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1183,8 +1177,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{37E64DA8-0107-43CB-81F5-E280262A46B8}" name="Tabla10" displayName="Tabla10" ref="G1:G6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="G1:G6" xr:uid="{37E64DA8-0107-43CB-81F5-E280262A46B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{37E64DA8-0107-43CB-81F5-E280262A46B8}" name="Tabla10" displayName="Tabla10" ref="G1:G5" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="G1:G5" xr:uid="{37E64DA8-0107-43CB-81F5-E280262A46B8}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{1FB7CA99-BE97-4002-B0CD-8127F2CDC399}" name="MIEMBROS" dataDxfId="12"/>
   </tableColumns>
@@ -1511,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5836246-8BCD-47E2-84AB-56902646E67F}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1536,7 @@
         <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1559,7 +1553,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1570,13 +1564,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1590,10 +1584,10 @@
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1606,11 +1600,11 @@
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>70</v>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1623,11 +1617,8 @@
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1635,10 +1626,10 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1649,7 +1640,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1660,7 +1651,7 @@
         <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1674,7 +1665,7 @@
         <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1688,7 +1679,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1704,10 +1695,10 @@
         <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1715,24 +1706,24 @@
         <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1746,7 +1737,7 @@
         <v>29</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1757,10 +1748,10 @@
         <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1768,13 +1759,13 @@
         <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1785,28 +1776,28 @@
         <v>39</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>